<commit_message>
rewriting project , moved old to _v001- - - WIP!!!
</commit_message>
<xml_diff>
--- a/reserch/SD READ SPEEDS.xlsx
+++ b/reserch/SD READ SPEEDS.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dropbox\_DEV\_projects\drum-set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\_DEV\_projects\drum_kit\project\reserch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F397034E-7C69-4E29-9509-97627A4FCC49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="10395" xr2:uid="{7564FC77-BC53-4014-BBA9-3F5006DB63B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,9 +61,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +85,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -254,10 +263,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -314,25 +324,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -341,21 +351,31 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2684,7 +2704,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2748,12 +2768,12 @@
         <v>317.51937900000001</v>
       </c>
       <c r="D3" s="6">
-        <f>B3/C3*1000/1024</f>
+        <f t="shared" ref="D3:D12" si="0">B3/C3*1000/1024</f>
         <v>1.2302398714378942E-2</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="13">
-        <f>B3/88200*1000</f>
+        <f t="shared" ref="F3:F12" si="1">B3/88200*1000</f>
         <v>4.5351473922902494E-2</v>
       </c>
       <c r="G3" s="20">
@@ -2766,10 +2786,10 @@
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="24">
-        <f>$J$1*2*B3/1024</f>
+        <f t="shared" ref="J3:J12" si="2">$J$1*2*B3/1024</f>
         <v>0.3125</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="33">
         <f>J3*1024/$K$1</f>
         <v>1.0850694444444445E-3</v>
       </c>
@@ -2782,29 +2802,29 @@
         <v>470.804596</v>
       </c>
       <c r="D4" s="6">
-        <f>B4/C4*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>1.6593933165427299E-2</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="13">
-        <f>B4/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>9.0702947845804988E-2</v>
       </c>
       <c r="G4" s="20">
-        <f t="shared" ref="G4:G12" si="0">F4/D4</f>
+        <f t="shared" ref="G4:G12" si="3">F4/D4</f>
         <v>5.4660306837188202</v>
       </c>
       <c r="H4" s="30">
-        <f t="shared" ref="H4:H12" si="1">IF((F4-1)/D4&gt;0,(F4-1)/D4,0)</f>
+        <f t="shared" ref="H4:H12" si="4">IF((F4-1)/D4&gt;0,(F4-1)/D4,0)</f>
         <v>0</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="24">
-        <f>$J$1*2*B4/1024</f>
+        <f t="shared" si="2"/>
         <v>0.625</v>
       </c>
-      <c r="K4" s="6">
-        <f t="shared" ref="K4:K12" si="2">J4*1024/$K$1</f>
+      <c r="K4" s="33">
+        <f t="shared" ref="K4:K12" si="5">J4*1024/$K$1</f>
         <v>2.170138888888889E-3</v>
       </c>
     </row>
@@ -2816,29 +2836,29 @@
         <v>619.479736</v>
       </c>
       <c r="D5" s="6">
-        <f>B5/C5*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>2.5222778231441617E-2</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="13">
-        <f>B5/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>0.18140589569160998</v>
       </c>
       <c r="G5" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.192145687800453</v>
       </c>
       <c r="H5" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="24">
-        <f>$J$1*2*B5/1024</f>
+        <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
-      <c r="K5" s="6">
-        <f t="shared" si="2"/>
+      <c r="K5" s="33">
+        <f t="shared" si="5"/>
         <v>4.340277777777778E-3</v>
       </c>
     </row>
@@ -2850,29 +2870,29 @@
         <v>735.10406499999999</v>
       </c>
       <c r="D6" s="6">
-        <f>B6/C6*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>4.2510987883055712E-2</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="13">
-        <f>B6/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>0.36281179138321995</v>
       </c>
       <c r="G6" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.5345415256235828</v>
       </c>
       <c r="H6" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I6" s="20"/>
       <c r="J6" s="24">
-        <f>$J$1*2*B6/1024</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="K6" s="6">
-        <f t="shared" si="2"/>
+      <c r="K6" s="33">
+        <f t="shared" si="5"/>
         <v>8.6805555555555559E-3</v>
       </c>
     </row>
@@ -2884,16 +2904,16 @@
         <v>810.76800500000002</v>
       </c>
       <c r="D7" s="6">
-        <f>B7/C7*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>7.7087403072843258E-2</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="13">
-        <f>B7/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>0.7256235827664399</v>
       </c>
       <c r="G7" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.4129981532879814</v>
       </c>
       <c r="H7" s="30">
@@ -2902,11 +2922,11 @@
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="24">
-        <f>$J$1*2*B7/1024</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="K7" s="6">
-        <f t="shared" si="2"/>
+      <c r="K7" s="33">
+        <f t="shared" si="5"/>
         <v>1.7361111111111112E-2</v>
       </c>
     </row>
@@ -2918,29 +2938,29 @@
         <v>854.75793499999997</v>
       </c>
       <c r="D8" s="6">
-        <f>B8/C8*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>0.14624023349955798</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="13">
-        <f>B8/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>1.4512471655328798</v>
       </c>
       <c r="G8" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.9237202430839009</v>
       </c>
       <c r="H8" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.0856567630839002</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="24">
-        <f>$J$1*2*B8/1024</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="K8" s="6">
-        <f t="shared" si="2"/>
+      <c r="K8" s="33">
+        <f t="shared" si="5"/>
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
@@ -2952,29 +2972,29 @@
         <v>878.96997099999999</v>
       </c>
       <c r="D9" s="9">
-        <f>B9/C9*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>0.28442382362115987</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="14">
-        <f>B9/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>2.9024943310657596</v>
       </c>
       <c r="G9" s="21">
-        <f t="shared" si="0"/>
+        <f>F9/D9</f>
         <v>10.204821432018141</v>
       </c>
       <c r="H9" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.68894154801814</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="25">
-        <f>$J$1*2*B9/1024</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K9" s="9">
-        <f t="shared" si="2"/>
+      <c r="K9" s="34">
+        <f t="shared" si="5"/>
         <v>6.9444444444444448E-2</v>
       </c>
     </row>
@@ -2986,29 +3006,29 @@
         <v>891</v>
       </c>
       <c r="D10" s="9">
-        <f>B10/C10*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>0.5611672278338945</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="14">
-        <f>B10/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>5.8049886621315192</v>
       </c>
       <c r="G10" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10.344489795918367</v>
       </c>
       <c r="H10" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.562489795918367</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="25">
-        <f>$J$1*2*B10/1024</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K10" s="9">
-        <f t="shared" si="2"/>
+      <c r="K10" s="34">
+        <f t="shared" si="5"/>
         <v>0.1388888888888889</v>
       </c>
     </row>
@@ -3020,29 +3040,29 @@
         <v>902.20263699999998</v>
       </c>
       <c r="D11" s="6">
-        <f>B11/C11*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>1.1083984450823547</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="13">
-        <f>B11/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>11.609977324263038</v>
       </c>
       <c r="G11" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10.474552157460316</v>
       </c>
       <c r="H11" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.5723495204603157</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="24">
-        <f>$J$1*2*B11/1024</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="K11" s="6">
-        <f t="shared" si="2"/>
+      <c r="K11" s="33">
+        <f t="shared" si="5"/>
         <v>0.27777777777777779</v>
       </c>
     </row>
@@ -3054,29 +3074,29 @@
         <v>908.60693400000002</v>
       </c>
       <c r="D12" s="12">
-        <f>B12/C12*1000/1024</f>
+        <f t="shared" si="0"/>
         <v>2.2011718435774119</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="15">
-        <f>B12/88200*1000</f>
+        <f t="shared" si="1"/>
         <v>23.219954648526077</v>
       </c>
       <c r="G12" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10.548905900408164</v>
       </c>
       <c r="H12" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.094602433408165</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="26">
-        <f>$J$1*2*B12/1024</f>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="K12" s="12">
-        <f t="shared" si="2"/>
+      <c r="K12" s="35">
+        <f t="shared" si="5"/>
         <v>0.55555555555555558</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP - more better goodest things also - fixed some bugs also - changed structure oh , and now player kidda works already
</commit_message>
<xml_diff>
--- a/reserch/SD READ SPEEDS.xlsx
+++ b/reserch/SD READ SPEEDS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\_DEV\_projects\drum_kit\project\reserch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F397034E-7C69-4E29-9509-97627A4FCC49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F972C9B6-D9BD-4625-936E-03D9AF6B5FC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="10395" xr2:uid="{7564FC77-BC53-4014-BBA9-3F5006DB63B9}"/>
   </bookViews>
@@ -60,8 +60,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -282,36 +283,18 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -370,6 +353,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2704,7 +2705,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2732,31 +2733,31 @@
         <v>294912</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="19" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:11" s="13" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="27" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="17" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2767,29 +2768,29 @@
       <c r="C3" s="5">
         <v>317.51937900000001</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="30">
         <f t="shared" ref="D3:D12" si="0">B3/C3*1000/1024</f>
         <v>1.2302398714378942E-2</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="13">
+      <c r="F3" s="31">
         <f t="shared" ref="F3:F12" si="1">B3/88200*1000</f>
         <v>4.5351473922902494E-2</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="14">
         <f>F3/D3</f>
         <v>3.6863927902040814</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="23">
         <f>IF((F3-1)/D3&gt;0,(F3-1)/D3,0)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="24">
+      <c r="I3" s="14"/>
+      <c r="J3" s="18">
         <f t="shared" ref="J3:J12" si="2">$J$1*2*B3/1024</f>
         <v>0.3125</v>
       </c>
-      <c r="K3" s="33">
+      <c r="K3" s="27">
         <f>J3*1024/$K$1</f>
         <v>1.0850694444444445E-3</v>
       </c>
@@ -2801,29 +2802,29 @@
       <c r="C4" s="5">
         <v>470.804596</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="30">
         <f t="shared" si="0"/>
         <v>1.6593933165427299E-2</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="13">
+      <c r="F4" s="31">
         <f t="shared" si="1"/>
         <v>9.0702947845804988E-2</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="14">
         <f t="shared" ref="G4:G12" si="3">F4/D4</f>
         <v>5.4660306837188202</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="24">
         <f t="shared" ref="H4:H12" si="4">IF((F4-1)/D4&gt;0,(F4-1)/D4,0)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="24">
+      <c r="I4" s="14"/>
+      <c r="J4" s="18">
         <f t="shared" si="2"/>
         <v>0.625</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="27">
         <f t="shared" ref="K4:K12" si="5">J4*1024/$K$1</f>
         <v>2.170138888888889E-3</v>
       </c>
@@ -2835,29 +2836,29 @@
       <c r="C5" s="5">
         <v>619.479736</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="30">
         <f t="shared" si="0"/>
         <v>2.5222778231441617E-2</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="13">
-        <f t="shared" si="1"/>
+      <c r="F5" s="31">
+        <f>B5/88200*1000</f>
         <v>0.18140589569160998</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="14">
         <f t="shared" si="3"/>
         <v>7.192145687800453</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="24">
+      <c r="I5" s="14"/>
+      <c r="J5" s="18">
         <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="27">
         <f t="shared" si="5"/>
         <v>4.340277777777778E-3</v>
       </c>
@@ -2869,29 +2870,29 @@
       <c r="C6" s="5">
         <v>735.10406499999999</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="30">
         <f t="shared" si="0"/>
         <v>4.2510987883055712E-2</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="13">
+      <c r="F6" s="31">
         <f t="shared" si="1"/>
         <v>0.36281179138321995</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="14">
         <f t="shared" si="3"/>
         <v>8.5345415256235828</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="24">
+      <c r="I6" s="14"/>
+      <c r="J6" s="18">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="27">
         <f t="shared" si="5"/>
         <v>8.6805555555555559E-3</v>
       </c>
@@ -2903,29 +2904,29 @@
       <c r="C7" s="5">
         <v>810.76800500000002</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="30">
         <f t="shared" si="0"/>
         <v>7.7087403072843258E-2</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="13">
+      <c r="F7" s="31">
         <f t="shared" si="1"/>
         <v>0.7256235827664399</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="14">
         <f t="shared" si="3"/>
         <v>9.4129981532879814</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="24">
         <f>IF((F7-1)/D7&gt;0,(F7-1)/D7,0)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="24">
+      <c r="I7" s="14"/>
+      <c r="J7" s="18">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="27">
         <f t="shared" si="5"/>
         <v>1.7361111111111112E-2</v>
       </c>
@@ -2937,97 +2938,97 @@
       <c r="C8" s="5">
         <v>854.75793499999997</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="30">
         <f t="shared" si="0"/>
         <v>0.14624023349955798</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="13">
+      <c r="F8" s="31">
         <f t="shared" si="1"/>
         <v>1.4512471655328798</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="14">
         <f t="shared" si="3"/>
         <v>9.9237202430839009</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="24">
         <f t="shared" si="4"/>
         <v>3.0856567630839002</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="24">
+      <c r="I8" s="14"/>
+      <c r="J8" s="18">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="27">
         <f t="shared" si="5"/>
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>256</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>878.96997099999999</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="32">
         <f t="shared" si="0"/>
         <v>0.28442382362115987</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="14">
+      <c r="E9" s="7"/>
+      <c r="F9" s="34">
         <f t="shared" si="1"/>
         <v>2.9024943310657596</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="15">
         <f>F9/D9</f>
         <v>10.204821432018141</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="25">
         <f t="shared" si="4"/>
         <v>6.68894154801814</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="25">
+      <c r="I9" s="15"/>
+      <c r="J9" s="19">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="28">
         <f t="shared" si="5"/>
         <v>6.9444444444444448E-2</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>512</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>891</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="32">
         <f t="shared" si="0"/>
         <v>0.5611672278338945</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="14">
+      <c r="E10" s="7"/>
+      <c r="F10" s="34">
         <f t="shared" si="1"/>
         <v>5.8049886621315192</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="15">
         <f t="shared" si="3"/>
         <v>10.344489795918367</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="25">
         <f t="shared" si="4"/>
         <v>8.562489795918367</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="25">
+      <c r="I10" s="15"/>
+      <c r="J10" s="19">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="28">
         <f t="shared" si="5"/>
         <v>0.1388888888888889</v>
       </c>
@@ -3039,63 +3040,63 @@
       <c r="C11" s="5">
         <v>902.20263699999998</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="30">
         <f t="shared" si="0"/>
         <v>1.1083984450823547</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="13">
+      <c r="F11" s="31">
         <f t="shared" si="1"/>
         <v>11.609977324263038</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="14">
         <f t="shared" si="3"/>
         <v>10.474552157460316</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="24">
         <f t="shared" si="4"/>
         <v>9.5723495204603157</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="24">
+      <c r="I11" s="14"/>
+      <c r="J11" s="18">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="K11" s="33">
+      <c r="K11" s="27">
         <f t="shared" si="5"/>
         <v>0.27777777777777779</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+      <c r="B12" s="8">
         <v>2048</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <v>908.60693400000002</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="33">
         <f t="shared" si="0"/>
         <v>2.2011718435774119</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="15">
+      <c r="E12" s="9"/>
+      <c r="F12" s="35">
         <f t="shared" si="1"/>
         <v>23.219954648526077</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="16">
         <f t="shared" si="3"/>
         <v>10.548905900408164</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="26">
         <f t="shared" si="4"/>
         <v>10.094602433408165</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="26">
+      <c r="I12" s="16"/>
+      <c r="J12" s="20">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="K12" s="35">
+      <c r="K12" s="29">
         <f t="shared" si="5"/>
         <v>0.55555555555555558</v>
       </c>

</xml_diff>